<commit_message>
Add our Viva problems here
</commit_message>
<xml_diff>
--- a/14.05.17/Problems&Solutions.xlsx
+++ b/14.05.17/Problems&Solutions.xlsx
@@ -49,9 +49,6 @@
     <t>1. Most probably today is our viva day.</t>
   </si>
   <si>
-    <t>2. Need do our best as individual and as a team.</t>
-  </si>
-  <si>
     <t>3. Not a big problem of presenting the facts since we can practice. But better if we can get an idea of problems they can ask</t>
   </si>
   <si>
@@ -59,6 +56,9 @@
   </si>
   <si>
     <t>5. Are we ready?</t>
+  </si>
+  <si>
+    <t>2. Need to do our best as individual and as a team.</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,22 +465,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add VIVA sample priblems here
</commit_message>
<xml_diff>
--- a/14.05.17/Problems&Solutions.xlsx
+++ b/14.05.17/Problems&Solutions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Problem</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>6. Reviews for 1st slide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. Do u think 140 characters for a tweet is enough to preserve the reliability? </t>
   </si>
 </sst>
 </file>
@@ -423,7 +426,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,6 +500,11 @@
         <v>17</v>
       </c>
     </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Add ur sample problems for VIVA here
</commit_message>
<xml_diff>
--- a/14.05.17/Problems&Solutions.xlsx
+++ b/14.05.17/Problems&Solutions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Problem</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">7. Do u think 140 characters for a tweet is enough to preserve the reliability? </t>
+  </si>
+  <si>
+    <t>8. Reviews for 2nd slide</t>
   </si>
 </sst>
 </file>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,13 +508,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add viva sample problems here
</commit_message>
<xml_diff>
--- a/14.05.17/Problems&Solutions.xlsx
+++ b/14.05.17/Problems&Solutions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Problem</t>
   </si>
@@ -74,6 +74,15 @@
   </si>
   <si>
     <t>8. Reviews for 2nd slide</t>
+  </si>
+  <si>
+    <t>9. Since I am the first speaker may be need a bit introduction. So I supposed to add an introduction slide</t>
+  </si>
+  <si>
+    <t>10. At the introduction do I need to tell the overview of presentation including everyone topics</t>
+  </si>
+  <si>
+    <t>11. I feel like need to change the order of 1st topic and 2nd topic. Since need to introduce the twitter in the 1st slide Anuradha can get</t>
   </si>
 </sst>
 </file>
@@ -426,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,13 +522,28 @@
         <v>19</v>
       </c>
     </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ur viva problems here
</commit_message>
<xml_diff>
--- a/14.05.17/Problems&Solutions.xlsx
+++ b/14.05.17/Problems&Solutions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Problem</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>11. I feel like need to change the order of 1st topic and 2nd topic. Since need to introduce the twitter in the 1st slide Anuradha can get</t>
+  </si>
+  <si>
+    <t>12. what I learnt from Twitter reliability to my softwares...</t>
+  </si>
+  <si>
+    <t>13. If I make a social media site what should I do to protect the reliability?</t>
   </si>
 </sst>
 </file>
@@ -435,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,11 +545,21 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>